<commit_message>
Sprint 2 upload with sprint 3 plannign
</commit_message>
<xml_diff>
--- a/Team1 - Project Report.xlsx
+++ b/Team1 - Project Report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonathan Morrone\Desktop\Stevens\SSW555_Project_Team1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{962C7F22-172F-4179-B8CB-197FF5B2D623}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50BDE578-DB8F-4A7B-A328-23B5C0789523}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3360" yWindow="3525" windowWidth="28800" windowHeight="15345" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11130" yWindow="3555" windowWidth="28800" windowHeight="15345" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="250">
   <si>
     <t>Initials</t>
   </si>
@@ -698,6 +698,99 @@
   </si>
   <si>
     <t>T29.02</t>
+  </si>
+  <si>
+    <t>US 16</t>
+  </si>
+  <si>
+    <t>Male Last Name</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Complete</t>
+  </si>
+  <si>
+    <t>T16.1</t>
+  </si>
+  <si>
+    <t>Find Last Name of Father</t>
+  </si>
+  <si>
+    <t>T16.2</t>
+  </si>
+  <si>
+    <t>Find children in family</t>
+  </si>
+  <si>
+    <t>T16.3</t>
+  </si>
+  <si>
+    <t>Compare Last Name of father and child if it is a son</t>
+  </si>
+  <si>
+    <t>US 15</t>
+  </si>
+  <si>
+    <t>Less than 15 Siblings</t>
+  </si>
+  <si>
+    <t>T15.1</t>
+  </si>
+  <si>
+    <t>Find family of indavidual</t>
+  </si>
+  <si>
+    <t>T15.2</t>
+  </si>
+  <si>
+    <t>find how many children are in the family</t>
+  </si>
+  <si>
+    <t>T15.3</t>
+  </si>
+  <si>
+    <t>check if the amount of children is less than 15</t>
+  </si>
+  <si>
+    <t>US 31</t>
+  </si>
+  <si>
+    <t>T31.1</t>
+  </si>
+  <si>
+    <t>Check if indavidual is living</t>
+  </si>
+  <si>
+    <t>T31.2</t>
+  </si>
+  <si>
+    <t>T31.3</t>
+  </si>
+  <si>
+    <t>check if the indavidaul is over 30</t>
+  </si>
+  <si>
+    <t>Check if married or has ever been married</t>
+  </si>
+  <si>
+    <t>US 32</t>
+  </si>
+  <si>
+    <t>Multiple Births</t>
+  </si>
+  <si>
+    <t>T32.1</t>
+  </si>
+  <si>
+    <t>T32.2</t>
+  </si>
+  <si>
+    <t>Check indavidual birth dates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Find any that are the same </t>
   </si>
 </sst>
 </file>
@@ -1011,12 +1104,6 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="11" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1031,6 +1118,12 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1532,30 +1625,30 @@
     </row>
     <row r="3" spans="3:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="4" spans="3:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D4" s="45" t="s">
+      <c r="D4" s="52" t="s">
         <v>157</v>
       </c>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="52"/>
+      <c r="G4" s="52"/>
     </row>
     <row r="5" spans="3:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D5" s="45"/>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="45"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="52"/>
+      <c r="F5" s="52"/>
+      <c r="G5" s="52"/>
     </row>
     <row r="6" spans="3:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D6" s="45"/>
-      <c r="E6" s="45"/>
-      <c r="F6" s="45"/>
-      <c r="G6" s="45"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="52"/>
+      <c r="F6" s="52"/>
+      <c r="G6" s="52"/>
     </row>
     <row r="7" spans="3:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D7" s="45"/>
-      <c r="E7" s="45"/>
-      <c r="F7" s="45"/>
-      <c r="G7" s="45"/>
+      <c r="D7" s="52"/>
+      <c r="E7" s="52"/>
+      <c r="F7" s="52"/>
+      <c r="G7" s="52"/>
     </row>
     <row r="8" spans="3:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D8" s="14"/>
@@ -1564,12 +1657,12 @@
       <c r="G8" s="15"/>
     </row>
     <row r="9" spans="3:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D9" s="46" t="s">
+      <c r="D9" s="53" t="s">
         <v>158</v>
       </c>
-      <c r="E9" s="46"/>
-      <c r="F9" s="46"/>
-      <c r="G9" s="46"/>
+      <c r="E9" s="53"/>
+      <c r="F9" s="53"/>
+      <c r="G9" s="53"/>
     </row>
     <row r="10" spans="3:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="11" spans="3:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1634,7 +1727,7 @@
       <c r="E15" s="20" t="s">
         <v>198</v>
       </c>
-      <c r="F15" s="47" t="s">
+      <c r="F15" s="45" t="s">
         <v>199</v>
       </c>
       <c r="G15" s="20" t="s">
@@ -2645,7 +2738,7 @@
   <dimension ref="A1:Z1006"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -8216,7 +8309,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J994"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
+    <sheetView zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
       <selection activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
@@ -8660,23 +8753,23 @@
       <c r="J21" s="36"/>
     </row>
     <row r="22" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="48"/>
-      <c r="B22" s="48"/>
-      <c r="C22" s="49"/>
-      <c r="D22" s="50"/>
-      <c r="E22" s="50"/>
-      <c r="F22" s="51"/>
-      <c r="G22" s="50"/>
-      <c r="H22" s="50"/>
-      <c r="I22" s="50"/>
-      <c r="J22" s="52"/>
+      <c r="A22" s="46"/>
+      <c r="B22" s="46"/>
+      <c r="C22" s="47"/>
+      <c r="D22" s="48"/>
+      <c r="E22" s="48"/>
+      <c r="F22" s="49"/>
+      <c r="G22" s="48"/>
+      <c r="H22" s="48"/>
+      <c r="I22" s="48"/>
+      <c r="J22" s="50"/>
     </row>
     <row r="23" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="37" t="s">
         <v>118</v>
       </c>
       <c r="B23" s="37"/>
-      <c r="C23" s="53" t="s">
+      <c r="C23" s="51" t="s">
         <v>201</v>
       </c>
       <c r="D23" s="38" t="s">
@@ -8696,7 +8789,7 @@
       <c r="B24" s="37" t="s">
         <v>209</v>
       </c>
-      <c r="C24" s="53" t="s">
+      <c r="C24" s="51" t="s">
         <v>210</v>
       </c>
       <c r="D24" s="38" t="s">
@@ -8716,7 +8809,7 @@
       <c r="B25" s="37" t="s">
         <v>213</v>
       </c>
-      <c r="C25" s="53" t="s">
+      <c r="C25" s="51" t="s">
         <v>211</v>
       </c>
       <c r="D25" s="38" t="s">
@@ -8736,7 +8829,7 @@
       <c r="B26" s="37" t="s">
         <v>214</v>
       </c>
-      <c r="C26" s="53" t="s">
+      <c r="C26" s="51" t="s">
         <v>212</v>
       </c>
       <c r="D26" s="38" t="s">
@@ -8753,7 +8846,7 @@
     </row>
     <row r="27" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="37"/>
-      <c r="C27" s="53"/>
+      <c r="C27" s="51"/>
       <c r="D27" s="38"/>
       <c r="E27" s="38"/>
       <c r="F27" s="38"/>
@@ -8767,7 +8860,7 @@
         <v>115</v>
       </c>
       <c r="B28" s="37"/>
-      <c r="C28" s="53" t="s">
+      <c r="C28" s="51" t="s">
         <v>215</v>
       </c>
       <c r="D28" s="38" t="s">
@@ -8787,7 +8880,7 @@
       <c r="B29" s="37" t="s">
         <v>216</v>
       </c>
-      <c r="C29" s="53" t="s">
+      <c r="C29" s="51" t="s">
         <v>210</v>
       </c>
       <c r="D29" s="38" t="s">
@@ -12768,7 +12861,7 @@
   <dimension ref="A1:J1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -12819,25 +12912,47 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="20"/>
+      <c r="A2" s="7" t="s">
+        <v>219</v>
+      </c>
       <c r="B2" s="20"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
+      <c r="C2" s="43" t="s">
+        <v>220</v>
+      </c>
+      <c r="D2" s="35" t="s">
+        <v>196</v>
+      </c>
+      <c r="E2" s="35" t="s">
+        <v>222</v>
+      </c>
+      <c r="F2" s="35">
+        <v>30</v>
+      </c>
+      <c r="G2" s="35">
+        <v>60</v>
+      </c>
       <c r="H2" s="35"/>
       <c r="I2" s="35">
         <v>90</v>
       </c>
-      <c r="J2" s="36"/>
+      <c r="J2" s="36" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="3" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20"/>
-      <c r="B3" s="20"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
+      <c r="B3" s="20" t="s">
+        <v>223</v>
+      </c>
+      <c r="C3" s="34" t="s">
+        <v>224</v>
+      </c>
+      <c r="D3" s="35" t="s">
+        <v>196</v>
+      </c>
+      <c r="E3" s="35" t="s">
+        <v>222</v>
+      </c>
       <c r="F3" s="38"/>
       <c r="G3" s="38"/>
       <c r="H3" s="38"/>
@@ -12846,10 +12961,18 @@
     </row>
     <row r="4" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="20"/>
-      <c r="B4" s="20"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
+      <c r="B4" s="20" t="s">
+        <v>225</v>
+      </c>
+      <c r="C4" s="34" t="s">
+        <v>226</v>
+      </c>
+      <c r="D4" s="35" t="s">
+        <v>196</v>
+      </c>
+      <c r="E4" s="35" t="s">
+        <v>222</v>
+      </c>
       <c r="F4" s="38"/>
       <c r="G4" s="38"/>
       <c r="H4" s="38"/>
@@ -12858,10 +12981,18 @@
     </row>
     <row r="5" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="20"/>
-      <c r="B5" s="20"/>
-      <c r="C5" s="34"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
+      <c r="B5" s="20" t="s">
+        <v>227</v>
+      </c>
+      <c r="C5" s="34" t="s">
+        <v>228</v>
+      </c>
+      <c r="D5" s="35" t="s">
+        <v>196</v>
+      </c>
+      <c r="E5" s="35" t="s">
+        <v>222</v>
+      </c>
       <c r="F5" s="38"/>
       <c r="G5" s="38"/>
       <c r="H5" s="38"/>
@@ -12869,23 +13000,47 @@
       <c r="J5" s="36"/>
     </row>
     <row r="6" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="20"/>
+      <c r="A6" s="20" t="s">
+        <v>229</v>
+      </c>
       <c r="B6" s="20"/>
-      <c r="C6" s="44"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
+      <c r="C6" s="44" t="s">
+        <v>230</v>
+      </c>
+      <c r="D6" s="35" t="s">
+        <v>196</v>
+      </c>
+      <c r="E6" s="35" t="s">
+        <v>222</v>
+      </c>
+      <c r="F6" s="38">
+        <v>30</v>
+      </c>
+      <c r="G6" s="38">
+        <v>60</v>
+      </c>
       <c r="H6" s="38"/>
-      <c r="I6" s="38"/>
-      <c r="J6" s="36"/>
+      <c r="I6" s="38">
+        <v>90</v>
+      </c>
+      <c r="J6" s="36" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="7" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20"/>
-      <c r="B7" s="20"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="35"/>
-      <c r="E7" s="35"/>
+      <c r="B7" s="20" t="s">
+        <v>231</v>
+      </c>
+      <c r="C7" s="34" t="s">
+        <v>232</v>
+      </c>
+      <c r="D7" s="35" t="s">
+        <v>196</v>
+      </c>
+      <c r="E7" s="35" t="s">
+        <v>222</v>
+      </c>
       <c r="F7" s="38"/>
       <c r="G7" s="38"/>
       <c r="H7" s="38"/>
@@ -12894,10 +13049,18 @@
     </row>
     <row r="8" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="37"/>
-      <c r="B8" s="37"/>
-      <c r="C8" s="34"/>
-      <c r="D8" s="38"/>
-      <c r="E8" s="38"/>
+      <c r="B8" s="37" t="s">
+        <v>233</v>
+      </c>
+      <c r="C8" s="34" t="s">
+        <v>234</v>
+      </c>
+      <c r="D8" s="35" t="s">
+        <v>196</v>
+      </c>
+      <c r="E8" s="35" t="s">
+        <v>222</v>
+      </c>
       <c r="F8" s="38"/>
       <c r="G8" s="38"/>
       <c r="H8" s="38"/>
@@ -12906,10 +13069,18 @@
     </row>
     <row r="9" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20"/>
-      <c r="B9" s="20"/>
-      <c r="C9" s="43"/>
-      <c r="D9" s="35"/>
-      <c r="E9" s="35"/>
+      <c r="B9" s="20" t="s">
+        <v>235</v>
+      </c>
+      <c r="C9" s="43" t="s">
+        <v>236</v>
+      </c>
+      <c r="D9" s="35" t="s">
+        <v>196</v>
+      </c>
+      <c r="E9" s="35" t="s">
+        <v>222</v>
+      </c>
       <c r="F9" s="35"/>
       <c r="G9" s="35"/>
       <c r="H9" s="38"/>
@@ -17055,7 +17226,7 @@
   <dimension ref="A1:J1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -17099,25 +17270,43 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="20"/>
+      <c r="A2" s="20" t="s">
+        <v>237</v>
+      </c>
       <c r="B2" s="20"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
+      <c r="C2" s="43" t="s">
+        <v>205</v>
+      </c>
+      <c r="D2" s="35" t="s">
+        <v>196</v>
+      </c>
+      <c r="E2" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="F2" s="35">
+        <v>40</v>
+      </c>
+      <c r="G2" s="35">
+        <v>90</v>
+      </c>
       <c r="H2" s="35"/>
-      <c r="I2" s="35">
-        <v>90</v>
-      </c>
+      <c r="I2" s="35"/>
       <c r="J2" s="36"/>
     </row>
     <row r="3" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20"/>
-      <c r="B3" s="20"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
+      <c r="B3" s="20" t="s">
+        <v>238</v>
+      </c>
+      <c r="C3" s="34" t="s">
+        <v>239</v>
+      </c>
+      <c r="D3" s="35" t="s">
+        <v>196</v>
+      </c>
+      <c r="E3" s="35" t="s">
+        <v>166</v>
+      </c>
       <c r="F3" s="38"/>
       <c r="G3" s="38"/>
       <c r="H3" s="38"/>
@@ -17126,10 +17315,18 @@
     </row>
     <row r="4" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="20"/>
-      <c r="B4" s="20"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
+      <c r="B4" s="20" t="s">
+        <v>240</v>
+      </c>
+      <c r="C4" s="34" t="s">
+        <v>243</v>
+      </c>
+      <c r="D4" s="35" t="s">
+        <v>196</v>
+      </c>
+      <c r="E4" s="35" t="s">
+        <v>166</v>
+      </c>
       <c r="F4" s="38"/>
       <c r="G4" s="38"/>
       <c r="H4" s="38"/>
@@ -17138,22 +17335,42 @@
     </row>
     <row r="5" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="20"/>
-      <c r="B5" s="20"/>
-      <c r="C5" s="34"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
+      <c r="B5" s="20" t="s">
+        <v>241</v>
+      </c>
+      <c r="C5" s="34" t="s">
+        <v>242</v>
+      </c>
+      <c r="D5" s="35" t="s">
+        <v>196</v>
+      </c>
+      <c r="E5" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="F5" s="38">
+        <v>20</v>
+      </c>
+      <c r="G5" s="38">
+        <v>45</v>
+      </c>
       <c r="H5" s="38"/>
       <c r="I5" s="38"/>
       <c r="J5" s="36"/>
     </row>
     <row r="6" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="20"/>
+      <c r="A6" s="20" t="s">
+        <v>244</v>
+      </c>
       <c r="B6" s="20"/>
-      <c r="C6" s="44"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
+      <c r="C6" s="44" t="s">
+        <v>245</v>
+      </c>
+      <c r="D6" s="35" t="s">
+        <v>196</v>
+      </c>
+      <c r="E6" s="35" t="s">
+        <v>166</v>
+      </c>
       <c r="F6" s="38"/>
       <c r="G6" s="38"/>
       <c r="H6" s="38"/>
@@ -17162,10 +17379,18 @@
     </row>
     <row r="7" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20"/>
-      <c r="B7" s="20"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="35"/>
-      <c r="E7" s="35"/>
+      <c r="B7" s="20" t="s">
+        <v>246</v>
+      </c>
+      <c r="C7" s="34" t="s">
+        <v>248</v>
+      </c>
+      <c r="D7" s="35" t="s">
+        <v>196</v>
+      </c>
+      <c r="E7" s="35" t="s">
+        <v>166</v>
+      </c>
       <c r="F7" s="38"/>
       <c r="G7" s="38"/>
       <c r="H7" s="38"/>
@@ -17174,10 +17399,18 @@
     </row>
     <row r="8" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="37"/>
-      <c r="B8" s="37"/>
-      <c r="C8" s="34"/>
-      <c r="D8" s="38"/>
-      <c r="E8" s="38"/>
+      <c r="B8" s="37" t="s">
+        <v>247</v>
+      </c>
+      <c r="C8" s="34" t="s">
+        <v>249</v>
+      </c>
+      <c r="D8" s="35" t="s">
+        <v>196</v>
+      </c>
+      <c r="E8" s="35" t="s">
+        <v>166</v>
+      </c>
       <c r="F8" s="38"/>
       <c r="G8" s="38"/>
       <c r="H8" s="38"/>
@@ -19791,7 +20024,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Final Sprint 2 report
</commit_message>
<xml_diff>
--- a/Team1 - Project Report.xlsx
+++ b/Team1 - Project Report.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\15513\Documents\Stevens Institute of Technology\Sem 3\SSW 555 Web Campus\Project\Project Assignment 5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\15513\Documents\Stevens Institute of Technology\Sem 3\SSW 555 Web Campus\Project\Project 6 Sprint - 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{760BE4B9-2A8A-44C6-9233-E684C00D00CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C52C564-D906-4AA9-8BEA-C45B52BB6EF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3465" yWindow="3465" windowWidth="16200" windowHeight="9308" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2573" yWindow="2573" windowWidth="16199" windowHeight="9307" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -4313,8 +4313,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A2:AA1001"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4426,11 +4426,16 @@
       <c r="D5" s="33">
         <v>8</v>
       </c>
-      <c r="E5" s="33"/>
+      <c r="E5" s="33">
+        <v>873</v>
+      </c>
       <c r="F5" s="33">
         <v>720</v>
       </c>
-      <c r="G5" s="36"/>
+      <c r="G5" s="36">
+        <f>(E5-E4)/F5*60</f>
+        <v>35.75</v>
+      </c>
     </row>
     <row r="6" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="33" t="s">
@@ -13067,7 +13072,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:J999"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>

</xml_diff>